<commit_message>
edit - changed the plots title and remove the plots with the previous title
</commit_message>
<xml_diff>
--- a/analyses/data/pilotData_100_kin.xlsx
+++ b/analyses/data/pilotData_100_kin.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27984" uniqueCount="13992">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59312" uniqueCount="13992">
   <si>
     <t>StimDuration</t>
   </si>
@@ -42009,7 +42009,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="320">
+  <borders count="1032">
     <border>
       <left/>
       <right/>
@@ -42336,11 +42336,723 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="320">
+  <cellXfs count="1032">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -42661,6 +43373,718 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="317" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="318" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="319" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="320" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="321" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="322" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="323" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="324" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="325" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="326" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="327" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="328" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="329" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="330" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="331" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="332" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="333" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="334" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="335" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="336" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="337" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="338" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="339" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="340" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="341" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="342" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="343" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="344" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="345" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="346" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="347" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="348" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="349" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="350" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="351" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="352" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="353" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="354" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="355" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="356" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="357" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="358" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="359" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="360" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="361" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="362" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="363" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="364" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="365" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="366" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="367" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="368" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="369" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="370" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="371" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="372" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="373" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="374" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="375" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="376" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="377" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="378" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="379" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="380" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="381" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="382" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="383" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="384" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="385" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="386" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="387" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="388" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="389" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="390" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="391" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="392" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="393" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="394" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="395" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="396" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="397" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="398" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="399" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="400" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="401" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="402" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="403" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="404" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="405" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="406" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="407" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="408" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="409" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="410" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="411" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="412" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="413" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="414" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="415" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="416" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="417" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="418" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="419" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="420" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="421" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="422" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="423" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="424" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="425" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="426" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="427" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="428" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="429" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="430" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="431" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="432" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="433" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="434" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="435" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="436" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="437" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="438" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="439" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="440" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="441" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="442" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="443" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="444" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="445" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="446" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="447" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="448" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="449" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="450" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="451" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="452" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="453" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="454" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="455" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="456" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="457" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="458" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="459" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="460" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="461" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="462" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="463" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="464" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="465" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="466" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="467" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="468" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="469" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="470" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="471" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="472" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="473" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="474" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="475" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="476" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="477" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="478" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="479" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="480" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="481" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="482" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="483" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="484" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="485" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="486" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="487" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="488" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="489" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="490" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="491" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="492" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="493" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="494" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="495" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="496" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="497" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="498" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="499" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="500" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="501" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="502" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="503" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="504" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="505" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="506" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="507" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="508" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="509" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="510" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="511" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="512" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="513" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="514" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="515" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="516" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="517" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="518" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="519" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="520" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="521" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="522" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="523" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="524" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="525" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="526" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="527" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="528" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="529" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="530" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="531" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="532" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="533" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="534" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="535" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="536" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="537" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="538" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="539" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="540" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="541" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="542" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="543" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="544" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="545" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="546" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="547" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="548" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="549" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="550" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="551" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="552" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="553" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="554" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="555" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="556" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="557" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="558" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="559" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="560" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="561" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="562" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="563" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="564" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="565" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="566" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="567" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="568" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="569" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="570" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="571" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="572" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="573" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="574" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="575" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="576" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="577" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="578" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="579" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="580" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="581" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="582" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="583" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="584" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="585" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="586" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="587" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="588" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="589" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="590" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="591" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="592" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="593" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="594" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="595" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="596" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="597" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="598" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="599" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="600" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="601" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="602" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="603" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="604" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="605" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="606" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="607" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="608" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="609" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="610" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="611" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="612" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="613" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="614" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="615" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="616" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="617" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="618" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="619" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="620" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="621" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="622" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="623" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="624" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="625" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="626" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="627" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="628" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="629" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="630" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="631" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="632" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="633" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="634" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="635" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="636" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="637" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="638" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="639" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="640" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="641" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="642" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="643" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="644" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="645" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="646" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="647" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="648" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="649" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="650" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="651" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="652" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="653" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="654" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="655" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="656" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="657" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="658" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="659" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="660" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="661" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="662" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="663" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="664" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="665" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="666" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="667" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="668" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="669" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="670" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="671" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="672" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="673" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="674" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="675" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="676" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="677" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="678" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="679" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="680" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="681" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="682" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="683" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="684" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="685" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="686" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="687" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="688" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="689" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="690" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="691" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="692" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="693" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="694" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="695" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="696" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="697" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="698" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="699" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="700" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="701" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="702" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="703" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="704" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="705" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="706" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="707" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="708" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="709" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="710" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="711" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="712" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="713" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="714" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="715" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="716" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="717" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="718" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="719" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="720" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="721" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="722" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="723" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="724" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="725" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="726" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="727" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="728" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="729" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="730" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="731" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="732" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="733" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="734" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="735" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="736" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="737" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="738" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="739" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="740" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="741" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="742" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="743" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="744" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="745" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="746" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="747" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="748" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="749" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="750" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="751" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="752" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="753" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="754" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="755" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="756" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="757" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="758" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="759" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="760" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="761" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="762" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="763" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="764" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="765" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="766" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="767" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="768" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="769" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="770" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="771" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="772" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="773" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="774" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="775" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="776" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="777" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="778" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="779" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="780" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="781" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="782" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="783" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="784" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="785" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="786" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="787" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="788" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="789" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="790" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="791" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="792" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="793" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="794" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="795" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="796" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="797" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="798" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="799" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="800" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="801" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="802" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="803" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="804" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="805" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="806" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="807" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="808" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="809" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="810" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="811" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="812" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="813" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="814" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="815" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="816" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="817" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="818" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="819" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="820" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="821" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="822" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="823" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="824" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="825" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="826" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="827" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="828" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="829" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="830" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="831" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="832" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="833" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="834" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="835" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="836" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="837" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="838" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="839" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="840" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="841" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="842" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="843" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="844" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="845" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="846" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="847" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="848" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="849" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="850" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="851" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="852" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="853" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="854" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="855" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="856" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="857" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="858" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="859" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="860" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="861" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="862" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="863" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="864" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="865" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="866" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="867" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="868" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="869" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="870" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="871" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="872" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="873" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="874" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="875" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="876" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="877" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="878" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="879" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="880" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="881" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="882" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="883" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="884" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="885" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="886" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="887" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="888" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="889" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="890" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="891" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="892" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="893" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="894" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="895" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="896" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="897" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="898" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="899" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="900" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="901" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="902" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="903" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="904" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="905" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="906" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="907" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="908" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="909" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="910" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="911" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="912" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="913" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="914" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="915" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="916" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="917" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="918" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="919" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="920" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="921" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="922" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="923" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="924" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="925" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="926" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="927" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="928" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="929" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="930" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="931" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="932" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="933" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="934" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="935" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="936" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="937" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="938" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="939" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="940" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="941" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="942" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="943" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="944" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="945" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="946" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="947" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="948" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="949" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="950" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="951" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="952" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="953" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="954" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="955" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="956" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="957" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="958" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="959" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="960" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="961" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="962" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="963" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="964" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="965" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="966" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="967" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="968" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="969" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="970" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="971" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="972" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="973" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="974" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="975" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="976" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="977" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="978" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="979" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="980" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="981" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="982" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="983" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="984" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="985" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="986" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="987" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="988" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="989" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="990" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="991" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="992" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="993" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="994" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="995" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="996" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="997" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="998" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="999" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1000" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1001" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1002" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1003" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1004" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1005" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1006" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1007" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1008" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1009" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1010" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1011" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1012" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1013" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1014" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1015" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1016" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1017" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1018" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1019" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1020" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1021" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1022" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1023" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1024" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1025" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1026" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1027" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1028" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1029" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1030" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1031" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -42764,268 +44188,268 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="318" t="s">
+      <c r="A1" s="1030" t="s">
         <v>13904</v>
       </c>
-      <c r="B1" s="318" t="s">
+      <c r="B1" s="1030" t="s">
         <v>13905</v>
       </c>
-      <c r="C1" s="318" t="s">
+      <c r="C1" s="1030" t="s">
         <v>13906</v>
       </c>
-      <c r="D1" s="318" t="s">
+      <c r="D1" s="1030" t="s">
         <v>13907</v>
       </c>
-      <c r="E1" s="318" t="s">
+      <c r="E1" s="1030" t="s">
         <v>13908</v>
       </c>
-      <c r="F1" s="318" t="s">
+      <c r="F1" s="1030" t="s">
         <v>13909</v>
       </c>
-      <c r="G1" s="318" t="s">
+      <c r="G1" s="1030" t="s">
         <v>13910</v>
       </c>
-      <c r="H1" s="318" t="s">
+      <c r="H1" s="1030" t="s">
         <v>13911</v>
       </c>
-      <c r="I1" s="318" t="s">
+      <c r="I1" s="1030" t="s">
         <v>13912</v>
       </c>
-      <c r="J1" s="318" t="s">
+      <c r="J1" s="1030" t="s">
         <v>13913</v>
       </c>
-      <c r="K1" s="318" t="s">
+      <c r="K1" s="1030" t="s">
         <v>13914</v>
       </c>
-      <c r="L1" s="318" t="s">
+      <c r="L1" s="1030" t="s">
         <v>13915</v>
       </c>
-      <c r="M1" s="318" t="s">
+      <c r="M1" s="1030" t="s">
         <v>13916</v>
       </c>
-      <c r="N1" s="318" t="s">
+      <c r="N1" s="1030" t="s">
         <v>13917</v>
       </c>
-      <c r="O1" s="318" t="s">
+      <c r="O1" s="1030" t="s">
         <v>13918</v>
       </c>
-      <c r="P1" s="318" t="s">
+      <c r="P1" s="1030" t="s">
         <v>13919</v>
       </c>
-      <c r="Q1" s="318" t="s">
+      <c r="Q1" s="1030" t="s">
         <v>13920</v>
       </c>
-      <c r="R1" s="318" t="s">
+      <c r="R1" s="1030" t="s">
         <v>13921</v>
       </c>
-      <c r="S1" s="318" t="s">
+      <c r="S1" s="1030" t="s">
         <v>13922</v>
       </c>
-      <c r="T1" s="318" t="s">
+      <c r="T1" s="1030" t="s">
         <v>13923</v>
       </c>
-      <c r="U1" s="318" t="s">
+      <c r="U1" s="1030" t="s">
         <v>13924</v>
       </c>
-      <c r="V1" s="318" t="s">
+      <c r="V1" s="1030" t="s">
         <v>13925</v>
       </c>
-      <c r="W1" s="318" t="s">
+      <c r="W1" s="1030" t="s">
         <v>13926</v>
       </c>
-      <c r="X1" s="318" t="s">
+      <c r="X1" s="1030" t="s">
         <v>13927</v>
       </c>
-      <c r="Y1" s="318" t="s">
+      <c r="Y1" s="1030" t="s">
         <v>13928</v>
       </c>
-      <c r="Z1" s="318" t="s">
+      <c r="Z1" s="1030" t="s">
         <v>13929</v>
       </c>
-      <c r="AA1" s="318" t="s">
+      <c r="AA1" s="1030" t="s">
         <v>13930</v>
       </c>
-      <c r="AB1" s="318" t="s">
+      <c r="AB1" s="1030" t="s">
         <v>13931</v>
       </c>
-      <c r="AC1" s="318" t="s">
+      <c r="AC1" s="1030" t="s">
         <v>13932</v>
       </c>
-      <c r="AD1" s="318" t="s">
+      <c r="AD1" s="1030" t="s">
         <v>13933</v>
       </c>
-      <c r="AE1" s="318" t="s">
+      <c r="AE1" s="1030" t="s">
         <v>13934</v>
       </c>
-      <c r="AF1" s="318" t="s">
+      <c r="AF1" s="1030" t="s">
         <v>13935</v>
       </c>
-      <c r="AG1" s="318" t="s">
+      <c r="AG1" s="1030" t="s">
         <v>13936</v>
       </c>
-      <c r="AH1" s="318" t="s">
+      <c r="AH1" s="1030" t="s">
         <v>13937</v>
       </c>
-      <c r="AI1" s="318" t="s">
+      <c r="AI1" s="1030" t="s">
         <v>13938</v>
       </c>
-      <c r="AJ1" s="318" t="s">
+      <c r="AJ1" s="1030" t="s">
         <v>13939</v>
       </c>
-      <c r="AK1" s="318" t="s">
+      <c r="AK1" s="1030" t="s">
         <v>13940</v>
       </c>
-      <c r="AL1" s="318" t="s">
+      <c r="AL1" s="1030" t="s">
         <v>13941</v>
       </c>
-      <c r="AM1" s="318" t="s">
+      <c r="AM1" s="1030" t="s">
         <v>13942</v>
       </c>
-      <c r="AN1" s="318" t="s">
+      <c r="AN1" s="1030" t="s">
         <v>13943</v>
       </c>
-      <c r="AO1" s="318" t="s">
+      <c r="AO1" s="1030" t="s">
         <v>13944</v>
       </c>
-      <c r="AP1" s="318" t="s">
+      <c r="AP1" s="1030" t="s">
         <v>13945</v>
       </c>
-      <c r="AQ1" s="318" t="s">
+      <c r="AQ1" s="1030" t="s">
         <v>13946</v>
       </c>
-      <c r="AR1" s="318" t="s">
+      <c r="AR1" s="1030" t="s">
         <v>13947</v>
       </c>
-      <c r="AS1" s="318" t="s">
+      <c r="AS1" s="1030" t="s">
         <v>13948</v>
       </c>
-      <c r="AT1" s="318" t="s">
+      <c r="AT1" s="1030" t="s">
         <v>13949</v>
       </c>
-      <c r="AU1" s="318" t="s">
+      <c r="AU1" s="1030" t="s">
         <v>13950</v>
       </c>
-      <c r="AV1" s="318" t="s">
+      <c r="AV1" s="1030" t="s">
         <v>13951</v>
       </c>
-      <c r="AW1" s="318" t="s">
+      <c r="AW1" s="1030" t="s">
         <v>13952</v>
       </c>
-      <c r="AX1" s="318" t="s">
+      <c r="AX1" s="1030" t="s">
         <v>13953</v>
       </c>
-      <c r="AY1" s="318" t="s">
+      <c r="AY1" s="1030" t="s">
         <v>13954</v>
       </c>
-      <c r="AZ1" s="318" t="s">
+      <c r="AZ1" s="1030" t="s">
         <v>13955</v>
       </c>
-      <c r="BA1" s="318" t="s">
+      <c r="BA1" s="1030" t="s">
         <v>13956</v>
       </c>
-      <c r="BB1" s="318" t="s">
+      <c r="BB1" s="1030" t="s">
         <v>13957</v>
       </c>
-      <c r="BC1" s="318" t="s">
+      <c r="BC1" s="1030" t="s">
         <v>13958</v>
       </c>
-      <c r="BD1" s="318" t="s">
+      <c r="BD1" s="1030" t="s">
         <v>13959</v>
       </c>
-      <c r="BE1" s="318" t="s">
+      <c r="BE1" s="1030" t="s">
         <v>13960</v>
       </c>
-      <c r="BF1" s="318" t="s">
+      <c r="BF1" s="1030" t="s">
         <v>13961</v>
       </c>
-      <c r="BG1" s="318" t="s">
+      <c r="BG1" s="1030" t="s">
         <v>13962</v>
       </c>
-      <c r="BH1" s="318" t="s">
+      <c r="BH1" s="1030" t="s">
         <v>13963</v>
       </c>
-      <c r="BI1" s="318" t="s">
+      <c r="BI1" s="1030" t="s">
         <v>13964</v>
       </c>
-      <c r="BJ1" s="318" t="s">
+      <c r="BJ1" s="1030" t="s">
         <v>13965</v>
       </c>
-      <c r="BK1" s="318" t="s">
+      <c r="BK1" s="1030" t="s">
         <v>13966</v>
       </c>
-      <c r="BL1" s="318" t="s">
+      <c r="BL1" s="1030" t="s">
         <v>13967</v>
       </c>
-      <c r="BM1" s="318" t="s">
+      <c r="BM1" s="1030" t="s">
         <v>13968</v>
       </c>
-      <c r="BN1" s="318" t="s">
+      <c r="BN1" s="1030" t="s">
         <v>13969</v>
       </c>
-      <c r="BO1" s="318" t="s">
+      <c r="BO1" s="1030" t="s">
         <v>13970</v>
       </c>
-      <c r="BP1" s="318" t="s">
+      <c r="BP1" s="1030" t="s">
         <v>13971</v>
       </c>
-      <c r="BQ1" s="318" t="s">
+      <c r="BQ1" s="1030" t="s">
         <v>13972</v>
       </c>
-      <c r="BR1" s="318" t="s">
+      <c r="BR1" s="1030" t="s">
         <v>13973</v>
       </c>
-      <c r="BS1" s="318" t="s">
+      <c r="BS1" s="1030" t="s">
         <v>13974</v>
       </c>
-      <c r="BT1" s="318" t="s">
+      <c r="BT1" s="1030" t="s">
         <v>13975</v>
       </c>
-      <c r="BU1" s="318" t="s">
+      <c r="BU1" s="1030" t="s">
         <v>13976</v>
       </c>
-      <c r="BV1" s="318" t="s">
+      <c r="BV1" s="1030" t="s">
         <v>13977</v>
       </c>
-      <c r="BW1" s="318" t="s">
+      <c r="BW1" s="1030" t="s">
         <v>13978</v>
       </c>
-      <c r="BX1" s="318" t="s">
+      <c r="BX1" s="1030" t="s">
         <v>13979</v>
       </c>
-      <c r="BY1" s="318" t="s">
+      <c r="BY1" s="1030" t="s">
         <v>13980</v>
       </c>
-      <c r="BZ1" s="318" t="s">
+      <c r="BZ1" s="1030" t="s">
         <v>13981</v>
       </c>
-      <c r="CA1" s="318" t="s">
+      <c r="CA1" s="1030" t="s">
         <v>13982</v>
       </c>
-      <c r="CB1" s="318" t="s">
+      <c r="CB1" s="1030" t="s">
         <v>13983</v>
       </c>
-      <c r="CC1" s="318" t="s">
+      <c r="CC1" s="1030" t="s">
         <v>13984</v>
       </c>
-      <c r="CD1" s="318" t="s">
+      <c r="CD1" s="1030" t="s">
         <v>13985</v>
       </c>
-      <c r="CE1" s="318" t="s">
+      <c r="CE1" s="1030" t="s">
         <v>13986</v>
       </c>
-      <c r="CF1" s="318" t="s">
+      <c r="CF1" s="1030" t="s">
         <v>13987</v>
       </c>
-      <c r="CG1" s="318" t="s">
+      <c r="CG1" s="1030" t="s">
         <v>13988</v>
       </c>
-      <c r="CH1" s="318" t="s">
+      <c r="CH1" s="1030" t="s">
         <v>13989</v>
       </c>
-      <c r="CI1" s="318" t="s">
+      <c r="CI1" s="1030" t="s">
         <v>13990</v>
       </c>
-      <c r="CJ1" s="318" t="s">
+      <c r="CJ1" s="1030" t="s">
         <v>13991</v>
       </c>
     </row>

</xml_diff>